<commit_message>
train log, add new datafile
</commit_message>
<xml_diff>
--- a/ensemble/ensemble.xlsx
+++ b/ensemble/ensemble.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming_Design\CCF-BDCI-fewshot-classification\ensemble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DD21AF-66A9-4F80-96B2-F063E32A6E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E379B6C8-7D67-4DBC-8846-93DBC21BF51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>2022_11_01_04_26_32-3-0.63293263685</t>
   </si>
@@ -91,13 +102,25 @@
   </si>
   <si>
     <t>2022_11_04_23_13_57</t>
+  </si>
+  <si>
+    <t>2022_11_05_09_09_13</t>
+  </si>
+  <si>
+    <t>2022_11_05_09_14_17</t>
+  </si>
+  <si>
+    <t>2022_11_02_19_58_44-3-0.62829439429</t>
+  </si>
+  <si>
+    <t>2022_11_05_09_26_44</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +135,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,6 +184,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -430,21 +472,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="10" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -466,8 +508,17 @@
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +540,17 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -512,8 +572,17 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -535,9 +604,18 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -558,8 +636,17 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -581,8 +668,17 @@
       <c r="G6" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -604,8 +700,17 @@
       <c r="G7" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -627,8 +732,17 @@
       <c r="G8" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -650,65 +764,152 @@
       <c r="G9" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="1">
         <v>0.63415516318999998</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>0.63234589688999998</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>0.62031840512000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="E11" s="1">
+        <v>0.63589020368000004</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.63438827984000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.63079113464000003</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.63685043782999995</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.62772075951999995</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.63410110356000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
+        <v>0.64228001062999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
train file and log
</commit_message>
<xml_diff>
--- a/ensemble/ensemble.xlsx
+++ b/ensemble/ensemble.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming_Design\CCF-BDCI-fewshot-classification\ensemble\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904D2ADA-31F9-4154-8A86-61FFC5731409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9CB6E8-6930-42CF-95A3-472B0FC12FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>2022_11_01_04_26_32-3-0.63293263685</t>
   </si>
@@ -128,10 +128,78 @@
     <t>2022_11_05_22_26_27</t>
   </si>
   <si>
-    <t>2022_11_05_22_26_38</t>
-  </si>
-  <si>
-    <t>2022_11_05_22_26_49</t>
+    <t>2022_11_06_14_31_56</t>
+  </si>
+  <si>
+    <t>2022_11_06_04_35_15-1-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_04_35_15-2-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_04_35_15-3-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_04_34_51_1</t>
+  </si>
+  <si>
+    <t>2022_11_06_04_34_51_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_04_34_51_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_14_54_03</t>
+  </si>
+  <si>
+    <t>2022_11_06_04_38_28_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_04_38_28_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_04_38_28_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_15_02_51</t>
+  </si>
+  <si>
+    <t>2022_11_06_04_37_58_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_04_37_58_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_04_37_58_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_16_22_30</t>
+  </si>
+  <si>
+    <t>2022_11_06_09_05_33_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_09_05_33_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_09_05_33_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022_11_06_19_51_17</t>
   </si>
 </sst>
 </file>
@@ -213,10 +281,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -499,24 +567,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomRight" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="15" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="18" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -560,10 +628,19 @@
         <v>27</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,8 +686,17 @@
       <c r="O2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -656,8 +742,17 @@
       <c r="O3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -703,8 +798,17 @@
       <c r="O4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -750,8 +854,17 @@
       <c r="O5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -795,10 +908,19 @@
         <v>1</v>
       </c>
       <c r="O6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -839,13 +961,22 @@
         <v>1</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -886,13 +1017,22 @@
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -938,35 +1078,20 @@
       <c r="O9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
       <c r="J10" s="1">
         <v>1</v>
       </c>
@@ -985,38 +1110,20 @@
       <c r="O10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
       <c r="K11" s="1">
         <v>1</v>
       </c>
@@ -1032,149 +1139,401 @@
       <c r="O11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="1">
+        <v>1</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="1">
+        <v>1</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P18" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B27" s="1">
         <v>0.63415516318999998</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C27" s="1">
         <v>0.63234589688999998</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D27" s="1">
         <v>0.62031840512000003</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E27" s="1">
         <v>0.63589020368000004</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F27" s="1">
         <v>0.63438827984000001</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G27" s="1">
         <v>0.63079113464000003</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H27" s="1">
         <v>0.63685043782999995</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I27" s="1">
         <v>0.62772075951999995</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J27" s="1">
         <v>0.63410110356000005</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K27" s="1">
         <v>0.64302561999999996</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L27" s="1">
         <v>0.63827990195999995</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M27" s="6">
         <v>0.63773401452</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="N27" s="5">
+        <v>0.63948215335000003</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0.63535529643999999</v>
+      </c>
+      <c r="P27" s="1">
+        <v>0.63471431104999998</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>0.63587641847999998</v>
+      </c>
+      <c r="R27" s="1">
+        <v>0.63115529438999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="P28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E15" s="1" t="s">
+      <c r="P29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E31" s="3">
         <v>0.64228001062999995</v>
       </c>
     </row>

</xml_diff>